<commit_message>
NEW: Add option to specify first column
</commit_message>
<xml_diff>
--- a/data/test/test.xlsx
+++ b/data/test/test.xlsx
@@ -4,11 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="140" windowWidth="14960" windowHeight="11180" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2700" yWindow="1620" windowWidth="19360" windowHeight="13020" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="test.csv" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="4" r:id="rId2"/>
+    <sheet name="sheet0" sheetId="1" r:id="rId1"/>
+    <sheet name="sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="sheet0_bad" sheetId="5" r:id="rId3"/>
+    <sheet name="sheet1_bad" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>Some Date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,14 +96,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
-    <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
-    <numFmt numFmtId="166" formatCode="mmmm\ d\,\ yyyy"/>
-    <numFmt numFmtId="167" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="168" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="169" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
-    <numFmt numFmtId="170" formatCode="hh:mm:ss\ AM/PM"/>
+  <numFmts count="13">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="170" formatCode="mm/dd/yy"/>
+    <numFmt numFmtId="171" formatCode="dd\-mmm\-yy"/>
+    <numFmt numFmtId="172" formatCode="mmmm\ d\,\ yyyy"/>
+    <numFmt numFmtId="173" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="174" formatCode="m/d/yyyy"/>
+    <numFmt numFmtId="175" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
+    <numFmt numFmtId="176" formatCode="hh:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -135,13 +143,13 @@
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="174" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -636,6 +644,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -650,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
   <cols>
@@ -774,6 +783,256 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="B2:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <cols>
+    <col min="2" max="3" width="16" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6">
+      <c r="B3" s="1">
+        <v>30075</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6">
+      <c r="B4" s="2">
+        <v>42005</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4" s="2"/>
+      <c r="F4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6">
+      <c r="B5" s="3">
+        <v>35064</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5">
+        <v>0.44</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6">
+      <c r="B7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="B2:J7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12"/>
+  <cols>
+    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="3" max="3" width="13.83203125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" customWidth="1"/>
+    <col min="8" max="9" width="24" customWidth="1"/>
+    <col min="10" max="10" width="45" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:10">
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="5">
+        <v>5844</v>
+      </c>
+      <c r="D3">
+        <v>164</v>
+      </c>
+      <c r="E3" s="8" t="b">
+        <f>FALSE</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>41800000.009999998</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>5844</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5">
+        <v>16071</v>
+      </c>
+      <c r="D4">
+        <v>63</v>
+      </c>
+      <c r="E4" s="8" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1.27</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.62306712962962962</v>
+      </c>
+      <c r="H4" s="6">
+        <v>16071.623067129629</v>
+      </c>
+      <c r="J4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5">
+        <v>24472</v>
+      </c>
+      <c r="D5">
+        <v>40</v>
+      </c>
+      <c r="E5" s="8" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.1763888888888889</v>
+      </c>
+      <c r="H5" s="6">
+        <v>24472.176388888889</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>